<commit_message>
Check cells for '  ' and similar whitespace only
</commit_message>
<xml_diff>
--- a/src/Food Journal.xlsx
+++ b/src/Food Journal.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dan\workspace\DansFoodJournal\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\working\DansFoodJournal\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -634,7 +634,7 @@
   <dimension ref="A1:I28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1035,13 +1035,13 @@
       <c r="G24" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="I24" s="2" t="s">
-        <v>82</v>
-      </c>
     </row>
     <row r="25" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <v>41248</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>82</v>
       </c>
       <c r="G25" s="2" t="s">
         <v>83</v>

</xml_diff>

<commit_message>
Commented out some debugging prints.
</commit_message>
<xml_diff>
--- a/src/Food Journal.xlsx
+++ b/src/Food Journal.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="120">
   <si>
     <t>Date</t>
   </si>
@@ -297,6 +297,93 @@
   </si>
   <si>
     <t>Tuna sandwich</t>
+  </si>
+  <si>
+    <t>Five Guys Burger;Fries;Water</t>
+  </si>
+  <si>
+    <t>Trail Mix</t>
+  </si>
+  <si>
+    <t>Veggie burger; Sweet potatoe fries</t>
+  </si>
+  <si>
+    <t>Chocolate</t>
+  </si>
+  <si>
+    <t>Oreos; Dorritos</t>
+  </si>
+  <si>
+    <t>Scrambled eggs; Bacon; Bagel with butter; Water</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Pulled pork wrap; Water</t>
+  </si>
+  <si>
+    <t>Chipoltle Burrito; Chips and Guac;Water</t>
+  </si>
+  <si>
+    <t>Scrambled eggs; Sausage; Bagel with butter; Waffle; Butter</t>
+  </si>
+  <si>
+    <t>Pasta with peas, corn, carrots, chicken, and alfredo sauce; Water</t>
+  </si>
+  <si>
+    <t>Rice Crispie Treat</t>
+  </si>
+  <si>
+    <t>Almonds</t>
+  </si>
+  <si>
+    <t>Scrambled eggs; Bacon; French toast; Water</t>
+  </si>
+  <si>
+    <t>Pulled chicken; Rice; Naan; Peas and mushrooms</t>
+  </si>
+  <si>
+    <t>Lamb over rice</t>
+  </si>
+  <si>
+    <t>Bagel with cream cheese</t>
+  </si>
+  <si>
+    <t>Chicken with rice and veggies</t>
+  </si>
+  <si>
+    <t>Gummy Bears</t>
+  </si>
+  <si>
+    <t>Pasta with chicken, veggies, and alfredo sauce</t>
+  </si>
+  <si>
+    <t>Scrambled eggs; Bagel with butter; French toast; Water</t>
+  </si>
+  <si>
+    <t>Pasta with peas, carrots, green &amp; red peppers, broccoli, chicken, and alfredo sauce; Cookies; Water</t>
+  </si>
+  <si>
+    <t>Pork; Mashed potatoes; Green beans; Pasta; Water</t>
+  </si>
+  <si>
+    <t>Cookies</t>
+  </si>
+  <si>
+    <t>Meatball sub; Salad; Chocolate cake; Water</t>
+  </si>
+  <si>
+    <t>Chicken Parm; Water</t>
+  </si>
+  <si>
+    <t>Scrambled eggs; Bacon; Oatmeal; Water</t>
+  </si>
+  <si>
+    <t>Baked Chicken;Mashed potatoes Veggies; Water</t>
+  </si>
+  <si>
+    <t>Chocolate croissant</t>
   </si>
 </sst>
 </file>
@@ -631,10 +718,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I28"/>
+  <dimension ref="A1:I39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1089,6 +1176,163 @@
         <v>90</v>
       </c>
     </row>
+    <row r="29" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+      <c r="A29" s="3">
+        <v>41252</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="I29" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A30" s="3">
+        <v>41253</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="I30" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+      <c r="A31" s="3">
+        <v>41254</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="H31" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A32" s="3">
+        <v>41255</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="A33" s="3">
+        <v>41256</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="H33" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="I33" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A34" s="3">
+        <v>41257</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="H34" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A35" s="3">
+        <v>41258</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="G35" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="H35" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="I35" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A36" s="3">
+        <v>41259</v>
+      </c>
+      <c r="G36" s="2" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+      <c r="A37" s="3">
+        <v>41260</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="G37" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="I37" s="2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A38" s="3">
+        <v>41261</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="G38" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A39" s="3">
+        <v>41262</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="G39" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="I39" s="2" t="s">
+        <v>119</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>